<commit_message>
Feat: Openpyxl 로 복귀 및 코드 완성
Pandas가 bool 값을 제대로 읽지 못하고 1/0 으로 읽는 앙증맞은 찐빠가 있었다! 앆!

엑셀 쪽을 내보내는 코드는 이제 완성했다.

남은건 json으로부터 템플릿을 가져오는 코드.

그리고 다른 이들도 쓸 수 있게 외장 꾸미기.
</commit_message>
<xml_diff>
--- a/test_XL.xlsx
+++ b/test_XL.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\카타클리즘_BN\NappingOcean의 모드들!\Py Support Tool\PyCata_XL_to_JSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A6D012-999B-43F2-B7AF-D9529A74F226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D266C4B9-380F-4D32-8C9A-B62F3632D754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31065" yWindow="-3420" windowWidth="11775" windowHeight="16560" xr2:uid="{F2874DB4-9BD3-4C56-A298-9DD50AC3BC7D}"/>
+    <workbookView xWindow="31065" yWindow="-3420" windowWidth="11775" windowHeight="16560" activeTab="1" xr2:uid="{F2874DB4-9BD3-4C56-A298-9DD50AC3BC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERIC" sheetId="5" r:id="rId1"/>
+    <sheet name="mutation" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +220,74 @@
   </si>
   <si>
     <t>CROWBAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>points</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>starting_trait</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vitamins_absorb_multi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flesh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vitA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancels:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CANNIBAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEATARIAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANTIFRUIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vitB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vitC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calcium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VEGETARIAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meat Intorlerance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You have problems with eating meat.  It's possible for you to eat it, but you will suffer morale penalties and obtain less nutrition from it.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5597971-5CDE-448B-AFF0-117442E1537E}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -796,4 +865,118 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDA907E-51ED-4401-85E2-B28FA7DE5589}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2">
+        <v>-2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>